<commit_message>
Encontrado que es obligatorio el campo empresa en el empleador
</commit_message>
<xml_diff>
--- a/src/java/com/sap/files/formato_empleadores.xlsx
+++ b/src/java/com/sap/files/formato_empleadores.xlsx
@@ -113,7 +113,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-OPCIONAL</t>
+OBLIGATORIO</t>
         </r>
       </text>
     </comment>
@@ -523,7 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>